<commit_message>
the pd.get_dummies function was reverted to OneHotEncoder
</commit_message>
<xml_diff>
--- a/src/output/summary/summary.xlsx
+++ b/src/output/summary/summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kensa\Dropbox\job hunting\freelance\yoshihiro_shin\Machine_Learning_Preprocessing_and_Performance_Test_after_Feature_Selection\Python\classification\output\summary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kensa\Dropbox\job hunting\freelance\yoshihiro_shin\Machine_Learning_Preprocessing_and_Performance_Test_after_Feature_Selection\src\output\summary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DFD2D0-CC7A-45F4-931A-27EFFCFF9646}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2289B23C-8ACB-48D0-9A2E-8865574A8298}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="-108" windowWidth="22248" windowHeight="13176" tabRatio="785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="-108" windowWidth="22248" windowHeight="13176" tabRatio="785" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
@@ -8510,7 +8510,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D10E3A13-8F89-4B6E-86AF-40AFF62AEFCF}">
   <dimension ref="B2:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="U29" sqref="U29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -49599,7 +49601,7 @@
         <v>99</v>
       </c>
       <c r="H2" t="str">
-        <f>IF(D2="naive_bayes", IF(E2=MAX($E$2:$E$7),"〇","×"),"×")</f>
+        <f t="shared" ref="H2:H7" si="0">IF(D2="naive_bayes", IF(E2=MAX($E$2:$E$7),"〇","×"),"×")</f>
         <v>×</v>
       </c>
       <c r="I2" t="s">
@@ -49629,7 +49631,7 @@
         <v>129</v>
       </c>
       <c r="H3" t="str">
-        <f>IF(D3="naive_bayes", IF(E3=MAX($E$2:$E$7),"〇","×"),"×")</f>
+        <f t="shared" si="0"/>
         <v>×</v>
       </c>
       <c r="I3" t="s">
@@ -49659,7 +49661,7 @@
         <v>162</v>
       </c>
       <c r="H4" t="str">
-        <f>IF(D4="naive_bayes", IF(E4=MAX($E$2:$E$7),"〇","×"),"×")</f>
+        <f t="shared" si="0"/>
         <v>×</v>
       </c>
       <c r="I4" t="s">
@@ -49689,7 +49691,7 @@
         <v>189</v>
       </c>
       <c r="H5" t="str">
-        <f>IF(D5="naive_bayes", IF(E5=MAX($E$2:$E$7),"〇","×"),"×")</f>
+        <f t="shared" si="0"/>
         <v>×</v>
       </c>
       <c r="I5" t="s">
@@ -49719,7 +49721,7 @@
         <v>218</v>
       </c>
       <c r="H6" t="str">
-        <f>IF(D6="naive_bayes", IF(E6=MAX($E$2:$E$7),"〇","×"),"×")</f>
+        <f t="shared" si="0"/>
         <v>〇</v>
       </c>
       <c r="I6" t="s">
@@ -49749,7 +49751,7 @@
         <v>237</v>
       </c>
       <c r="H7" t="str">
-        <f>IF(D7="naive_bayes", IF(E7=MAX($E$2:$E$7),"〇","×"),"×")</f>
+        <f t="shared" si="0"/>
         <v>×</v>
       </c>
       <c r="I7" t="s">
@@ -49809,7 +49811,7 @@
         <v>408</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" ref="H9:H13" si="0">IF(D9="naive_bayes", IF(E9=MAX($E$8:$E$13),"〇","×"),"×")</f>
+        <f t="shared" ref="H9:H13" si="1">IF(D9="naive_bayes", IF(E9=MAX($E$8:$E$13),"〇","×"),"×")</f>
         <v>×</v>
       </c>
       <c r="I9" t="s">
@@ -49839,7 +49841,7 @@
         <v>408</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>×</v>
       </c>
       <c r="I10" t="s">
@@ -49869,7 +49871,7 @@
         <v>408</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>〇</v>
       </c>
       <c r="I11" t="s">
@@ -49899,7 +49901,7 @@
         <v>408</v>
       </c>
       <c r="H12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>×</v>
       </c>
       <c r="I12" t="s">
@@ -49929,7 +49931,7 @@
         <v>401</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>×</v>
       </c>
       <c r="I13" t="s">
@@ -49959,7 +49961,7 @@
         <v>535</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" ref="H14:H19" si="1">IF(D14="naive_bayes", IF(E14=MAX($E$14:$E$19),"〇","×"),"×")</f>
+        <f t="shared" ref="H14:H19" si="2">IF(D14="naive_bayes", IF(E14=MAX($E$14:$E$19),"〇","×"),"×")</f>
         <v>×</v>
       </c>
       <c r="I14" t="s">
@@ -49989,7 +49991,7 @@
         <v>507</v>
       </c>
       <c r="H15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>×</v>
       </c>
       <c r="I15" t="s">
@@ -50019,7 +50021,7 @@
         <v>542</v>
       </c>
       <c r="H16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>×</v>
       </c>
       <c r="I16" t="s">
@@ -50049,7 +50051,7 @@
         <v>552</v>
       </c>
       <c r="H17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>×</v>
       </c>
       <c r="I17" t="s">
@@ -50079,7 +50081,7 @@
         <v>464</v>
       </c>
       <c r="H18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>×</v>
       </c>
       <c r="I18" t="s">
@@ -50109,7 +50111,7 @@
         <v>555</v>
       </c>
       <c r="H19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>〇</v>
       </c>
       <c r="I19" t="s">
@@ -50169,7 +50171,7 @@
         <v>645</v>
       </c>
       <c r="H21" t="str">
-        <f t="shared" ref="H21:H25" si="2">IF(D21="naive_bayes", IF(E21=MAX($E$20:$E$25),"〇","×"),"×")</f>
+        <f t="shared" ref="H21:H25" si="3">IF(D21="naive_bayes", IF(E21=MAX($E$20:$E$25),"〇","×"),"×")</f>
         <v>×</v>
       </c>
       <c r="I21" t="s">
@@ -50199,7 +50201,7 @@
         <v>655</v>
       </c>
       <c r="H22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>×</v>
       </c>
       <c r="I22" t="s">
@@ -50229,7 +50231,7 @@
         <v>642</v>
       </c>
       <c r="H23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>×</v>
       </c>
       <c r="I23" t="s">
@@ -50259,7 +50261,7 @@
         <v>664</v>
       </c>
       <c r="H24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>×</v>
       </c>
       <c r="I24" t="s">
@@ -50289,7 +50291,7 @@
         <v>672</v>
       </c>
       <c r="H25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>〇</v>
       </c>
       <c r="I25" t="s">
@@ -50349,7 +50351,7 @@
         <v>793</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" ref="H27:H31" si="3">IF(D27="naive_bayes", IF(E27=MAX($E$26:$E$31),"〇","×"),"×")</f>
+        <f t="shared" ref="H27:H31" si="4">IF(D27="naive_bayes", IF(E27=MAX($E$26:$E$31),"〇","×"),"×")</f>
         <v>×</v>
       </c>
       <c r="I27" t="s">
@@ -50379,7 +50381,7 @@
         <v>868</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>×</v>
       </c>
       <c r="I28" t="s">
@@ -50409,7 +50411,7 @@
         <v>888</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>×</v>
       </c>
       <c r="I29" t="s">
@@ -50439,7 +50441,7 @@
         <v>904</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>×</v>
       </c>
       <c r="I30" t="s">
@@ -50469,7 +50471,7 @@
         <v>921</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>〇</v>
       </c>
       <c r="I31" t="s">
@@ -50562,7 +50564,7 @@
         <v>1113</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" ref="H39:H43" si="4">IF(D39="naive_bayes", IF(E39=MAX($E$38:$E$43),"〇","×"),"×")</f>
+        <f t="shared" ref="H39:H43" si="5">IF(D39="naive_bayes", IF(E39=MAX($E$38:$E$43),"〇","×"),"×")</f>
         <v>×</v>
       </c>
       <c r="I39" t="s">
@@ -50592,7 +50594,7 @@
         <v>1113</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>×</v>
       </c>
       <c r="I40" t="s">
@@ -50622,7 +50624,7 @@
         <v>1131</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>×</v>
       </c>
       <c r="I41" t="s">
@@ -50652,7 +50654,7 @@
         <v>1135</v>
       </c>
       <c r="H42" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>×</v>
       </c>
       <c r="I42" t="s">
@@ -50682,7 +50684,7 @@
         <v>1144</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>×</v>
       </c>
       <c r="I43" t="s">
@@ -50712,7 +50714,7 @@
         <v>1269</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" ref="H44:H49" si="5">IF(D44="naive_bayes", IF(E44=MAX($E$44:$E$49),"〇","×"),"×")</f>
+        <f t="shared" ref="H44:H49" si="6">IF(D44="naive_bayes", IF(E44=MAX($E$44:$E$49),"〇","×"),"×")</f>
         <v>〇</v>
       </c>
       <c r="I44" t="s">
@@ -50742,7 +50744,7 @@
         <v>1269</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>〇</v>
       </c>
       <c r="I45" t="s">
@@ -50772,7 +50774,7 @@
         <v>1269</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>〇</v>
       </c>
       <c r="I46" t="s">
@@ -50802,7 +50804,7 @@
         <v>1269</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>〇</v>
       </c>
       <c r="I47" t="s">
@@ -50832,7 +50834,7 @@
         <v>1269</v>
       </c>
       <c r="H48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>〇</v>
       </c>
       <c r="I48" t="s">
@@ -50862,7 +50864,7 @@
         <v>1282</v>
       </c>
       <c r="H49" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>×</v>
       </c>
       <c r="I49" t="s">
@@ -50922,7 +50924,7 @@
         <v>1381</v>
       </c>
       <c r="H51" t="str">
-        <f t="shared" ref="H51:H55" si="6">IF(D51="naive_bayes", IF(E51=MAX($E$50:$E$55),"〇","×"),"×")</f>
+        <f t="shared" ref="H51:H55" si="7">IF(D51="naive_bayes", IF(E51=MAX($E$50:$E$55),"〇","×"),"×")</f>
         <v>×</v>
       </c>
       <c r="I51" t="s">
@@ -50952,7 +50954,7 @@
         <v>1397</v>
       </c>
       <c r="H52" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>×</v>
       </c>
       <c r="I52" t="s">
@@ -50982,7 +50984,7 @@
         <v>1408</v>
       </c>
       <c r="H53" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>×</v>
       </c>
       <c r="I53" t="s">
@@ -51012,7 +51014,7 @@
         <v>1333</v>
       </c>
       <c r="H54" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>×</v>
       </c>
       <c r="I54" t="s">
@@ -51042,7 +51044,7 @@
         <v>1423</v>
       </c>
       <c r="H55" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>〇</v>
       </c>
       <c r="I55" t="s">
@@ -51102,7 +51104,7 @@
         <v>1475</v>
       </c>
       <c r="H57" t="str">
-        <f t="shared" ref="H57:H61" si="7">IF(D57="naive_bayes", IF(E57=MAX($E$56:$E$61),"〇","×"),"×")</f>
+        <f t="shared" ref="H57:H61" si="8">IF(D57="naive_bayes", IF(E57=MAX($E$56:$E$61),"〇","×"),"×")</f>
         <v>〇</v>
       </c>
       <c r="I57" t="s">
@@ -51132,7 +51134,7 @@
         <v>1475</v>
       </c>
       <c r="H58" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>〇</v>
       </c>
       <c r="I58" t="s">
@@ -51162,7 +51164,7 @@
         <v>1475</v>
       </c>
       <c r="H59" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>〇</v>
       </c>
       <c r="I59" t="s">
@@ -51192,7 +51194,7 @@
         <v>1475</v>
       </c>
       <c r="H60" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>〇</v>
       </c>
       <c r="I60" t="s">
@@ -51222,7 +51224,7 @@
         <v>1475</v>
       </c>
       <c r="H61" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>〇</v>
       </c>
       <c r="I61" t="s">
@@ -51282,7 +51284,7 @@
         <v>1540</v>
       </c>
       <c r="H63" t="str">
-        <f t="shared" ref="H63:H67" si="8">IF(D63="naive_bayes", IF(E63=MAX($E$62:$E$67),"〇","×"),"×")</f>
+        <f t="shared" ref="H63:H67" si="9">IF(D63="naive_bayes", IF(E63=MAX($E$62:$E$67),"〇","×"),"×")</f>
         <v>×</v>
       </c>
       <c r="I63" t="s">
@@ -51312,7 +51314,7 @@
         <v>1546</v>
       </c>
       <c r="H64" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>×</v>
       </c>
       <c r="I64" t="s">
@@ -51342,7 +51344,7 @@
         <v>1546</v>
       </c>
       <c r="H65" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>×</v>
       </c>
       <c r="I65" t="s">
@@ -51372,7 +51374,7 @@
         <v>1546</v>
       </c>
       <c r="H66" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>〇</v>
       </c>
       <c r="I66" t="s">
@@ -51402,7 +51404,7 @@
         <v>1546</v>
       </c>
       <c r="H67" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>×</v>
       </c>
       <c r="I67" t="s">
@@ -51462,7 +51464,7 @@
         <v>1655</v>
       </c>
       <c r="H69" t="str">
-        <f t="shared" ref="H69:H73" si="9">IF(D69="naive_bayes", IF(E69=MAX($E$68:$E$73),"〇","×"),"×")</f>
+        <f t="shared" ref="H69:H73" si="10">IF(D69="naive_bayes", IF(E69=MAX($E$68:$E$73),"〇","×"),"×")</f>
         <v>×</v>
       </c>
       <c r="I69" t="s">
@@ -51492,7 +51494,7 @@
         <v>1665</v>
       </c>
       <c r="H70" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>〇</v>
       </c>
       <c r="I70" t="s">
@@ -51522,7 +51524,7 @@
         <v>1673</v>
       </c>
       <c r="H71" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>×</v>
       </c>
       <c r="I71" t="s">
@@ -51552,7 +51554,7 @@
         <v>1685</v>
       </c>
       <c r="H72" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>×</v>
       </c>
       <c r="I72" t="s">
@@ -51582,7 +51584,7 @@
         <v>1695</v>
       </c>
       <c r="H73" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>×</v>
       </c>
       <c r="I73" t="s">
@@ -56103,7 +56105,7 @@
         <v>0.73432835820895503</v>
       </c>
       <c r="H68" t="str">
-        <f>IF(D68="SVC", IF(E68=MAX($E$68:$E$73),"〇","×"),"×")</f>
+        <f t="shared" ref="H68:H73" si="10">IF(D68="SVC", IF(E68=MAX($E$68:$E$73),"〇","×"),"×")</f>
         <v>×</v>
       </c>
       <c r="I68" t="s">
@@ -56130,7 +56132,7 @@
         <v>0.78241619228336501</v>
       </c>
       <c r="H69" t="str">
-        <f>IF(D69="SVC", IF(E69=MAX($E$68:$E$73),"〇","×"),"×")</f>
+        <f t="shared" si="10"/>
         <v>×</v>
       </c>
       <c r="I69" t="s">
@@ -56157,7 +56159,7 @@
         <v>0.84591977869986101</v>
       </c>
       <c r="H70" t="str">
-        <f>IF(D70="SVC", IF(E70=MAX($E$68:$E$73),"〇","×"),"×")</f>
+        <f t="shared" si="10"/>
         <v>×</v>
       </c>
       <c r="I70" t="s">
@@ -56184,7 +56186,7 @@
         <v>0.88026607538802604</v>
       </c>
       <c r="H71" t="str">
-        <f>IF(D71="SVC", IF(E71=MAX($E$68:$E$73),"〇","×"),"×")</f>
+        <f t="shared" si="10"/>
         <v>×</v>
       </c>
       <c r="I71" t="s">
@@ -56211,7 +56213,7 @@
         <v>0.91345616973757604</v>
       </c>
       <c r="H72" t="str">
-        <f>IF(D72="SVC", IF(E72=MAX($E$68:$E$73),"〇","×"),"×")</f>
+        <f t="shared" si="10"/>
         <v>×</v>
       </c>
       <c r="I72" t="s">
@@ -56238,7 +56240,7 @@
         <v>0.93653899916130801</v>
       </c>
       <c r="H73" t="str">
-        <f>IF(D73="SVC", IF(E73=MAX($E$68:$E$73),"〇","×"),"×")</f>
+        <f t="shared" si="10"/>
         <v>〇</v>
       </c>
       <c r="I73" t="s">
@@ -56292,7 +56294,7 @@
         <v>0.76254681647940004</v>
       </c>
       <c r="H75" t="str">
-        <f t="shared" ref="H75:H79" si="10">IF(D75="SVC", IF(E75=MAX($E$74:$E$79),"〇","×"),"×")</f>
+        <f t="shared" ref="H75:H79" si="11">IF(D75="SVC", IF(E75=MAX($E$74:$E$79),"〇","×"),"×")</f>
         <v>×</v>
       </c>
       <c r="I75" t="s">
@@ -56319,7 +56321,7 @@
         <v>0.87714481811942302</v>
       </c>
       <c r="H76" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>×</v>
       </c>
       <c r="I76" t="s">
@@ -56346,7 +56348,7 @@
         <v>0.89413351314902201</v>
       </c>
       <c r="H77" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>×</v>
       </c>
       <c r="I77" t="s">
@@ -56373,7 +56375,7 @@
         <v>0.92838874680306904</v>
       </c>
       <c r="H78" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>×</v>
       </c>
       <c r="I78" t="s">
@@ -56400,7 +56402,7 @@
         <v>0.93466085874299898</v>
       </c>
       <c r="H79" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>〇</v>
       </c>
       <c r="I79" t="s">
@@ -56472,9 +56474,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3:I74"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -56586,7 +56588,7 @@
         <v>0.636750483558994</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" ref="H3:I8" si="0">IF(D4="naive_bayes", IF(E4=MAX($E$2:$E$7),"〇","×"),"×")</f>
+        <f t="shared" ref="H4:H7" si="0">IF(D4="naive_bayes", IF(E4=MAX($E$2:$E$7),"〇","×"),"×")</f>
         <v>×</v>
       </c>
       <c r="I4" t="s">
@@ -56721,7 +56723,7 @@
         <v>0.24</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" ref="H9:I13" si="1">IF(D9="naive_bayes", IF(E9=MAX($E$8:$E$13),"〇","×"),"×")</f>
+        <f t="shared" ref="H9:H13" si="1">IF(D9="naive_bayes", IF(E9=MAX($E$8:$E$13),"〇","×"),"×")</f>
         <v>×</v>
       </c>
       <c r="I9" t="s">
@@ -56856,7 +56858,7 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" ref="H14:I19" si="2">IF(D14="naive_bayes", IF(E14=MAX($E$14:$E$19),"〇","×"),"×")</f>
+        <f t="shared" ref="H14:H19" si="2">IF(D14="naive_bayes", IF(E14=MAX($E$14:$E$19),"〇","×"),"×")</f>
         <v>〇</v>
       </c>
       <c r="I14" t="s">
@@ -57045,7 +57047,7 @@
         <v>0.70512820512820495</v>
       </c>
       <c r="H21" t="str">
-        <f t="shared" ref="H21:I25" si="3">IF(D21="naive_bayes", IF(E21=MAX($E$20:$E$25),"〇","×"),"×")</f>
+        <f t="shared" ref="H21:H25" si="3">IF(D21="naive_bayes", IF(E21=MAX($E$20:$E$25),"〇","×"),"×")</f>
         <v>×</v>
       </c>
       <c r="I21" t="s">
@@ -57207,7 +57209,7 @@
         <v>0.52340425531914803</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" ref="H27:I31" si="4">IF(D27="naive_bayes", IF(E27=MAX($E$26:$E$31),"〇","×"),"×")</f>
+        <f t="shared" ref="H27:H31" si="4">IF(D27="naive_bayes", IF(E27=MAX($E$26:$E$31),"〇","×"),"×")</f>
         <v>×</v>
       </c>
       <c r="I27" t="s">
@@ -57402,7 +57404,7 @@
         <v>0.17708333333333301</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" ref="H39:I43" si="5">IF(D39="naive_bayes", IF(E39=MAX($E$38:$E$43),"〇","×"),"×")</f>
+        <f t="shared" ref="H39:H43" si="5">IF(D39="naive_bayes", IF(E39=MAX($E$38:$E$43),"〇","×"),"×")</f>
         <v>×</v>
       </c>
       <c r="I39" t="s">
@@ -57537,7 +57539,7 @@
         <v>0.58336334173568605</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" ref="H44:I49" si="6">IF(D44="naive_bayes", IF(E44=MAX($E$44:$E$49),"〇","×"),"×")</f>
+        <f t="shared" ref="H44:H49" si="6">IF(D44="naive_bayes", IF(E44=MAX($E$44:$E$49),"〇","×"),"×")</f>
         <v>×</v>
       </c>
       <c r="I44" t="s">
@@ -57726,7 +57728,7 @@
         <v>0.65961078866507294</v>
       </c>
       <c r="H51" t="str">
-        <f t="shared" ref="H51:I55" si="7">IF(D51="naive_bayes", IF(E51=MAX($E$50:$E$55),"〇","×"),"×")</f>
+        <f t="shared" ref="H51:H55" si="7">IF(D51="naive_bayes", IF(E51=MAX($E$50:$E$55),"〇","×"),"×")</f>
         <v>〇</v>
       </c>
       <c r="I51" t="s">
@@ -57888,7 +57890,7 @@
         <v>1</v>
       </c>
       <c r="H57" t="str">
-        <f t="shared" ref="H57:I61" si="8">IF(D57="naive_bayes", IF(E57=MAX($E$56:$E$61),"〇","×"),"×")</f>
+        <f t="shared" ref="H57:H61" si="8">IF(D57="naive_bayes", IF(E57=MAX($E$56:$E$61),"〇","×"),"×")</f>
         <v>〇</v>
       </c>
       <c r="I57" t="s">
@@ -58050,7 +58052,7 @@
         <v>0</v>
       </c>
       <c r="H63" t="str">
-        <f t="shared" ref="H63:I67" si="9">IF(D63="naive_bayes", IF(E63=MAX($E$62:$E$67),"〇","×"),"×")</f>
+        <f t="shared" ref="H63:H67" si="9">IF(D63="naive_bayes", IF(E63=MAX($E$62:$E$67),"〇","×"),"×")</f>
         <v>×</v>
       </c>
       <c r="I63" t="s">
@@ -58212,7 +58214,7 @@
         <v>0.78154425612052703</v>
       </c>
       <c r="H69" t="str">
-        <f t="shared" ref="H69:I79" si="10">IF(D69="naive_bayes", IF(E69=MAX($E$68:$E$73),"〇","×"),"×")</f>
+        <f t="shared" ref="H69:H72" si="10">IF(D69="naive_bayes", IF(E69=MAX($E$68:$E$73),"〇","×"),"×")</f>
         <v>〇</v>
       </c>
       <c r="I69" t="s">
@@ -58401,7 +58403,7 @@
         <v>0.62495111458740704</v>
       </c>
       <c r="H76" t="str">
-        <f t="shared" ref="H75:I79" si="11">IF(D76="naive_bayes", IF(E76=MAX($E$74:$E$79),"〇","×"),"×")</f>
+        <f t="shared" ref="H76:H79" si="11">IF(D76="naive_bayes", IF(E76=MAX($E$74:$E$79),"〇","×"),"×")</f>
         <v>×</v>
       </c>
       <c r="I76" t="s">

</xml_diff>